<commit_message>
creating and updating metadata templates in R
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-nutrient-transect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF74068-E733-AD45-9E9B-16EF0D4BCEF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB87746-56C9-BF4F-819C-ADE51F05FC19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
   <si>
     <t>attributeName</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t>0000-0002-4591-2842</t>
-  </si>
-  <si>
-    <t>principal investigator</t>
   </si>
   <si>
     <t>NSF</t>
@@ -954,10 +951,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9F15A2-54C5-8A40-9C46-AA79FB7AA201}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1017,131 +1014,99 @@
         <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
         <v>79</v>
       </c>
       <c r="I2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" t="s">
         <v>83</v>
-      </c>
-      <c r="J2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
         <v>79</v>
       </c>
-      <c r="E3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" t="s">
-        <v>81</v>
-      </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H3" t="s">
         <v>79</v>
       </c>
       <c r="I3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J3" t="s">
         <v>83</v>
-      </c>
-      <c r="J3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
         <v>79</v>
       </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H4" t="s">
         <v>79</v>
       </c>
       <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s">
         <v>83</v>
-      </c>
-      <c r="J4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>93</v>
       </c>
       <c r="D5" t="s">
         <v>79</v>
       </c>
-      <c r="E5" t="s">
-        <v>90</v>
+      <c r="E5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" t="s">
+        <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="H5" t="s">
         <v>79</v>
       </c>
       <c r="I5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" t="s">
         <v>83</v>
-      </c>
-      <c r="J5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" xr:uid="{FFBE1641-3BBE-8C40-923E-712A9E668498}"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{FFBE1641-3BBE-8C40-923E-712A9E668498}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1184,7 +1149,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1273,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1CE91A-BB2D-1F4C-8F3E-17163AD88A05}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
revisions to metadata and parent project
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-nutrient-transect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB87746-56C9-BF4F-819C-ADE51F05FC19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F3B6CA-CA12-9746-BF14-FF869B252A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27820" yWindow="460" windowWidth="30660" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="96">
   <si>
     <t>attributeName</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Lowercase letter indicating replicate subsample drawn from the same rosette bottle</t>
   </si>
   <si>
-    <t>Date and time of rosette bottle sample in UTC</t>
-  </si>
-  <si>
     <t>Ship's latitude when rosette bottle closed</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>keywordThesaurus</t>
   </si>
   <si>
-    <t>inorganic matter</t>
-  </si>
-  <si>
     <t>LTER Core Research Areas</t>
   </si>
   <si>
@@ -319,6 +313,9 @@
   </si>
   <si>
     <t>metadataProvider</t>
+  </si>
+  <si>
+    <t>Date and time in UTC when rosette bottle closed</t>
   </si>
 </sst>
 </file>
@@ -655,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -751,7 +748,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -771,7 +768,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -791,7 +788,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -953,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9F15A2-54C5-8A40-9C46-AA79FB7AA201}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -964,144 +961,144 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>73</v>
-      </c>
-      <c r="I1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" t="s">
         <v>76</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>79</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" t="s">
         <v>80</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>81</v>
-      </c>
-      <c r="G2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
         <v>85</v>
       </c>
-      <c r="C3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
       <c r="H3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s">
         <v>88</v>
       </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" t="s">
-        <v>90</v>
-      </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
         <v>91</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>93</v>
       </c>
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" t="s">
         <v>94</v>
       </c>
-      <c r="F5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G5" t="s">
-        <v>96</v>
-      </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1116,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8891376B-2E72-9645-AC2E-5AA2D44D3942}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1127,66 +1124,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -1194,23 +1191,23 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1218,15 +1215,15 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1246,19 +1243,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1266,16 +1263,16 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2">
         <v>1E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addition of student cruises to dataset
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-nutrient-transect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F3B6CA-CA12-9746-BF14-FF869B252A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A9C738-7655-6043-A0D1-9292A9477E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27820" yWindow="460" windowWidth="30660" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,7 +653,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
integration of python script to compile cruise data
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-nutrient-transect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A9C738-7655-6043-A0D1-9292A9477E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A384F0-0680-6347-9E83-C15C72EFA1FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27820" yWindow="460" windowWidth="30660" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
-    <sheet name="Personnel" sheetId="2" r:id="rId2"/>
-    <sheet name="Keywords" sheetId="3" r:id="rId3"/>
-    <sheet name="CustomUnits" sheetId="4" r:id="rId4"/>
+    <sheet name="CategoricalVariables" sheetId="5" r:id="rId2"/>
+    <sheet name="Personnel" sheetId="2" r:id="rId3"/>
+    <sheet name="Keywords" sheetId="3" r:id="rId4"/>
+    <sheet name="CustomUnits" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="113">
   <si>
     <t>attributeName</t>
   </si>
@@ -316,13 +317,64 @@
   </si>
   <si>
     <t>Date and time in UTC when rosette bottle closed</t>
+  </si>
+  <si>
+    <t>Nearest station is provided per cruise</t>
+  </si>
+  <si>
+    <t>nearest_station</t>
+  </si>
+  <si>
+    <t>alternate_sample_id</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>station_distance</t>
+  </si>
+  <si>
+    <t>kilometer</t>
+  </si>
+  <si>
+    <t>Sample identifier for project other than LTER</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>LTER</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>Long-Term Ecological Research</t>
+  </si>
+  <si>
+    <t>MIT-WHOI Joint Program</t>
+  </si>
+  <si>
+    <t>categorical</t>
+  </si>
+  <si>
+    <t>Distance from sample location to nearest station</t>
+  </si>
+  <si>
+    <t>Project associated with the sample collected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +386,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -360,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -369,6 +428,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -650,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -940,6 +1000,77 @@
         <v>8</v>
       </c>
     </row>
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -947,6 +1078,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCAFBFD-7807-F942-BC99-46AECE857774}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9F15A2-54C5-8A40-9C46-AA79FB7AA201}">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -1109,7 +1288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8891376B-2E72-9645-AC2E-5AA2D44D3942}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -1231,7 +1410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1CE91A-BB2D-1F4C-8F3E-17163AD88A05}">
   <dimension ref="A1:E2"/>
   <sheetViews>

</xml_diff>

<commit_message>
specifying use of python script
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-nutrient-transect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A384F0-0680-6347-9E83-C15C72EFA1FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9117AFAB-C5E3-684E-915E-D7389F207062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -136,9 +136,6 @@
     <t>meter</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
-  </si>
-  <si>
     <t>NaN</t>
   </si>
   <si>
@@ -368,6 +365,9 @@
   </si>
   <si>
     <t>Project associated with the sample collected</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD hh:mm:ss+hh:mm</t>
   </si>
 </sst>
 </file>
@@ -713,7 +713,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -757,7 +757,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -777,7 +777,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -797,7 +797,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -808,16 +808,16 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -828,7 +828,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -837,7 +837,7 @@
         <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -848,7 +848,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -857,7 +857,7 @@
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -877,7 +877,7 @@
         <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -888,7 +888,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -897,7 +897,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -908,13 +908,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -931,10 +931,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -951,10 +951,10 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -971,10 +971,10 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -991,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -1002,16 +1002,16 @@
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -1019,16 +1019,16 @@
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>8</v>
@@ -1036,16 +1036,16 @@
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -1053,19 +1053,19 @@
     </row>
     <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>8</v>
@@ -1089,35 +1089,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>104</v>
-      </c>
-      <c r="C1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1140,144 +1140,144 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>72</v>
-      </c>
-      <c r="J1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>76</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>78</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
         <v>79</v>
       </c>
-      <c r="G2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>80</v>
-      </c>
-      <c r="J2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
         <v>83</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" t="s">
-        <v>85</v>
-      </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
         <v>80</v>
-      </c>
-      <c r="J3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
         <v>86</v>
       </c>
-      <c r="D4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>87</v>
       </c>
-      <c r="G4" t="s">
-        <v>88</v>
-      </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" t="s">
         <v>80</v>
-      </c>
-      <c r="J4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
         <v>89</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>90</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" t="s">
         <v>92</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>93</v>
       </c>
-      <c r="G5" t="s">
-        <v>94</v>
-      </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" t="s">
         <v>80</v>
-      </c>
-      <c r="J5" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1303,66 +1303,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -1370,23 +1370,23 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1394,15 +1394,15 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
         <v>54</v>
-      </c>
-      <c r="B13" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1422,36 +1422,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
       <c r="D2">
         <v>1E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revisions to abstract and ammonium attribute
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-nutrient-transect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9117AFAB-C5E3-684E-915E-D7389F207062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D253FD10-0259-CA42-A7BB-52EE89038B3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,9 +115,6 @@
     <t>Identifier for research cruise generally including abbreviation for research vessel and voyage number</t>
   </si>
   <si>
-    <t>Ammonium concentration in the water column. Does not exactly match URI http://vocab.nerc.ac.uk/collection/P02/current/AMON/</t>
-  </si>
-  <si>
     <t>Phosphate concentration in the water column. URI http://vocab.nerc.ac.uk/collection/P02/current/PHOS/</t>
   </si>
   <si>
@@ -368,6 +365,9 @@
   </si>
   <si>
     <t>YYYY-MM-DD hh:mm:ss+hh:mm</t>
+  </si>
+  <si>
+    <t>Ammonium concentration in the water column</t>
   </si>
 </sst>
 </file>
@@ -713,7 +713,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -757,7 +757,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -777,7 +777,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -797,7 +797,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -808,16 +808,16 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -828,16 +828,16 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -848,16 +848,16 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -868,16 +868,16 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -888,7 +888,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -897,7 +897,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -908,13 +908,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -925,36 +925,36 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -965,16 +965,16 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -985,16 +985,16 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -1002,16 +1002,16 @@
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -1019,16 +1019,16 @@
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>8</v>
@@ -1036,16 +1036,16 @@
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -1053,19 +1053,19 @@
     </row>
     <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>8</v>
@@ -1089,35 +1089,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>103</v>
-      </c>
-      <c r="C1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1140,144 +1140,144 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
         <v>73</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>74</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>75</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>76</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>77</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" t="s">
         <v>78</v>
       </c>
-      <c r="G2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>79</v>
-      </c>
-      <c r="J2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
         <v>82</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
         <v>83</v>
       </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" t="s">
-        <v>84</v>
-      </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" t="s">
         <v>79</v>
-      </c>
-      <c r="J3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
         <v>85</v>
       </c>
-      <c r="D4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>86</v>
       </c>
-      <c r="G4" t="s">
-        <v>87</v>
-      </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" t="s">
         <v>79</v>
-      </c>
-      <c r="J4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" t="s">
         <v>91</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>92</v>
       </c>
-      <c r="G5" t="s">
-        <v>93</v>
-      </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" t="s">
         <v>79</v>
-      </c>
-      <c r="J5" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1303,66 +1303,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
         <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -1370,23 +1370,23 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1394,15 +1394,15 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s">
         <v>53</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1422,36 +1422,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>58</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
         <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
       </c>
       <c r="D2">
         <v>1E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revisions to methods section
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-nutrient-transect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D253FD10-0259-CA42-A7BB-52EE89038B3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69CA1C5-1781-E44D-844B-0495AF0D0114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -364,10 +364,10 @@
     <t>Project associated with the sample collected</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss+hh:mm</t>
-  </si>
-  <si>
     <t>Ammonium concentration in the water column</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
 </sst>
 </file>
@@ -713,7 +713,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -814,7 +814,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -945,7 +945,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
col rename attribute -> attributeName in CategoricalVariables sheet
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-nutrient-transect/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69CA1C5-1781-E44D-844B-0495AF0D0114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB55EBC-CCA7-4F23-B62E-E5CAD69502FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
   <si>
     <t>attributeName</t>
   </si>
@@ -332,9 +332,6 @@
   </si>
   <si>
     <t>Sample identifier for project other than LTER</t>
-  </si>
-  <si>
-    <t>attribute</t>
   </si>
   <si>
     <t>code</t>
@@ -712,18 +709,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="62.83203125" style="1" customWidth="1"/>
-    <col min="3" max="8" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="62.81640625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -763,7 +760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -783,7 +780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -803,7 +800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -814,7 +811,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -823,7 +820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -843,7 +840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -863,7 +860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -883,7 +880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -903,7 +900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -920,7 +917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -940,12 +937,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -960,7 +957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -980,7 +977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1000,7 +997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1017,15 +1014,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>97</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>34</v>
@@ -1034,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -1051,12 +1048,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>98</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1081,43 +1078,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCAFBFD-7807-F942-BC99-46AECE857774}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>101</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1133,12 +1128,12 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1170,7 +1165,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1202,7 +1197,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1225,7 +1220,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -1248,7 +1243,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1296,12 +1291,12 @@
       <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1309,7 +1304,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1317,7 +1312,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -1325,7 +1320,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -1333,7 +1328,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>46</v>
       </c>
@@ -1341,7 +1336,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
@@ -1349,7 +1344,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
@@ -1357,7 +1352,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -1365,7 +1360,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1373,7 +1368,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
@@ -1381,7 +1376,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -1389,7 +1384,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1397,7 +1392,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -1418,9 +1413,9 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1437,7 +1432,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
renamed distance_km -> station_distance, reran workflow
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6716AE0-22DC-4A0E-B1EC-E31418630C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6B88C7-C01B-4B6A-9DF9-1368F1F6F17E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
   <si>
     <t>attributeName</t>
   </si>
@@ -364,13 +364,7 @@
     <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
   <si>
-    <t>OOI</t>
-  </si>
-  <si>
-    <t>Ocean Observatories Initiative</t>
-  </si>
-  <si>
-    <t>distance_km</t>
+    <t>station_distance</t>
   </si>
 </sst>
 </file>
@@ -716,7 +710,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1056,7 +1050,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>107</v>
@@ -1082,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCAFBFD-7807-F942-BC99-46AECE857774}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1121,17 +1115,6 @@
       </c>
       <c r="C3" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Joe update keyword acknowledge OOI and JP
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfutrelle\Documents\GitHub\nes-lter-nutrient-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6B88C7-C01B-4B6A-9DF9-1368F1F6F17E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14724" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="118">
   <si>
     <t>attributeName</t>
   </si>
@@ -365,12 +364,30 @@
   </si>
   <si>
     <t>station_distance</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Futrelle</t>
+  </si>
+  <si>
+    <t>jfutrelle@whoi.edu</t>
+  </si>
+  <si>
+    <t>0000-0003-4537-5853</t>
+  </si>
+  <si>
+    <t>softwareDeveloper</t>
+  </si>
+  <si>
+    <t>inorganic matter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -706,21 +723,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="62.81640625" style="1" customWidth="1"/>
-    <col min="3" max="8" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="62.77734375" style="1" customWidth="1"/>
+    <col min="3" max="8" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -743,7 +760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -760,7 +777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -780,7 +797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -800,7 +817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -820,7 +837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -840,7 +857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -860,7 +877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -880,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -900,7 +917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -917,7 +934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -937,7 +954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -957,7 +974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -977,7 +994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -997,7 +1014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1014,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -1031,7 +1048,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -1048,7 +1065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -1075,16 +1092,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCAFBFD-7807-F942-BC99-46AECE857774}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1112,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1106,7 +1123,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1123,19 +1140,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9F15A2-54C5-8A40-9C46-AA79FB7AA201}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1167,7 +1184,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -1199,7 +1216,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1222,7 +1239,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -1245,27 +1262,24 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="D5" t="s">
         <v>75</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="H5" t="s">
         <v>75</v>
@@ -1277,28 +1291,61 @@
         <v>79</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{FFBE1641-3BBE-8C40-923E-712A9E668498}"/>
+    <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8891376B-2E72-9645-AC2E-5AA2D44D3942}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1306,15 +1353,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -1322,7 +1369,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -1330,7 +1377,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>46</v>
       </c>
@@ -1338,7 +1385,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>47</v>
       </c>
@@ -1346,7 +1393,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
@@ -1354,7 +1401,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>49</v>
       </c>
@@ -1362,7 +1409,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1370,7 +1417,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
@@ -1378,7 +1425,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -1386,7 +1433,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1394,7 +1441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -1408,16 +1455,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1CE91A-BB2D-1F4C-8F3E-17163AD88A05}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1434,7 +1481,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Taylor Emily creator AMON refrigerate
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60B179E-9FB3-4AB7-A77F-9EE01CF16C0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14724" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14724" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="120">
   <si>
     <t>attributeName</t>
   </si>
@@ -114,18 +115,9 @@
     <t>Identifier for research cruise generally including abbreviation for research vessel and voyage number</t>
   </si>
   <si>
-    <t>Phosphate concentration in the water column. URI http://vocab.nerc.ac.uk/collection/P02/current/PHOS/</t>
-  </si>
-  <si>
-    <t>Silicate concentration in the water column. URI http://vocab.nerc.ac.uk/collection/P02/current/SLCA/</t>
-  </si>
-  <si>
     <t>Depth of sample below sea surface. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
   </si>
   <si>
-    <t>Nitrate+nitrite concentration in the water column. URI http://vocab.nerc.ac.uk/collection/P02/current/NTRA/</t>
-  </si>
-  <si>
     <t>degree</t>
   </si>
   <si>
@@ -279,9 +271,6 @@
     <t>Crockford</t>
   </si>
   <si>
-    <t>technician</t>
-  </si>
-  <si>
     <t>NES-LTER Information Manager</t>
   </si>
   <si>
@@ -300,9 +289,6 @@
     <t>Wolfe</t>
   </si>
   <si>
-    <t>jawolfe@whoi.edu</t>
-  </si>
-  <si>
     <t>0000-0001-9620-5382</t>
   </si>
   <si>
@@ -357,9 +343,6 @@
     <t>Project associated with the sample collected</t>
   </si>
   <si>
-    <t>Ammonium concentration in the water column</t>
-  </si>
-  <si>
     <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
   <si>
@@ -382,12 +365,36 @@
   </si>
   <si>
     <t>inorganic matter</t>
+  </si>
+  <si>
+    <t>Ammonium concentration in the water column http://vocab.nerc.ac.uk/collection/P02/current/AMON/</t>
+  </si>
+  <si>
+    <t>Nitrate+nitrite concentration in the water column http://vocab.nerc.ac.uk/collection/P02/current/NTRA/</t>
+  </si>
+  <si>
+    <t>Phosphate concentration in the water column http://vocab.nerc.ac.uk/collection/P02/current/PHOS/</t>
+  </si>
+  <si>
+    <t>Silicate concentration in the water column http://vocab.nerc.ac.uk/collection/P02/current/SLCA/</t>
+  </si>
+  <si>
+    <t>epeacock@whoi.edu</t>
+  </si>
+  <si>
+    <t>ecrockford@whoi.edu</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Peacock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -723,11 +730,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +778,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -791,7 +798,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -811,7 +818,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -822,16 +829,16 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -842,16 +849,16 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -862,16 +869,16 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -882,16 +889,16 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -902,7 +909,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -911,7 +918,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -922,13 +929,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -939,36 +946,36 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -979,16 +986,16 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -999,16 +1006,16 @@
         <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -1016,16 +1023,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -1033,16 +1040,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>8</v>
@@ -1050,16 +1057,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -1067,19 +1074,19 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>8</v>
@@ -1092,7 +1099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1106,32 +1113,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
         <v>97</v>
       </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1140,11 +1147,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1154,189 +1161,215 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>68</v>
-      </c>
-      <c r="H1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>74</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" t="s">
         <v>75</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
         <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" t="s">
         <v>75</v>
       </c>
-      <c r="G3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" t="s">
-        <v>78</v>
-      </c>
       <c r="J3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
+        <v>119</v>
       </c>
       <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
         <v>75</v>
       </c>
-      <c r="E4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I4" t="s">
-        <v>78</v>
-      </c>
       <c r="J4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I5" t="s">
-        <v>78</v>
-      </c>
       <c r="J5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" t="s">
         <v>87</v>
       </c>
-      <c r="B6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="H7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I6" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" t="s">
-        <v>79</v>
+      <c r="J7" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1347,66 +1380,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1414,23 +1447,23 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1438,15 +1471,15 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1455,7 +1488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1466,36 +1499,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>1E-3</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ediutilities dependencies and fix errors
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-nutrient-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkoch\Desktop\LTER\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60B179E-9FB3-4AB7-A77F-9EE01CF16C0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411D9301-84F7-4855-B59C-7819F7BCE1A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14724" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="121">
   <si>
     <t>attributeName</t>
   </si>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t>Peacock</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -733,18 +736,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="62.77734375" style="1" customWidth="1"/>
-    <col min="3" max="8" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.41796875" customWidth="1"/>
+    <col min="2" max="2" width="62.7890625" style="1" customWidth="1"/>
+    <col min="3" max="8" width="20.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -767,7 +770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -784,7 +787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -804,7 +807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -824,7 +827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -844,7 +847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -864,7 +867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -884,7 +887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -904,7 +907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -924,7 +927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -941,7 +944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -961,7 +964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -975,13 +978,13 @@
         <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1021,7 +1024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>92</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>105</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>93</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>8</v>
@@ -1106,9 +1109,9 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -1150,16 +1153,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1223,7 +1226,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>118</v>
       </c>
@@ -1275,7 +1278,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -1298,7 +1301,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -1373,12 +1376,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -1410,7 +1413,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1418,7 +1421,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
@@ -1434,7 +1437,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
@@ -1442,7 +1445,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>47</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1495,9 +1498,9 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
update methods & missing value code
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466D3650-15AA-44A2-864F-CC7A4039590A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270DA7FA-5606-449E-953C-4A6975F2A6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="115">
   <si>
     <t>attributeName</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>Identifier for project that funded the cruise (or sample when available)</t>
+  </si>
+  <si>
+    <t>Distance to nearest station is greater than 2 km</t>
   </si>
 </sst>
 </file>
@@ -714,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1088,7 +1091,7 @@
         <v>31</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>8</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
rename date col, set nearest_station >2km to na
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270DA7FA-5606-449E-953C-4A6975F2A6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8CF89C-18C3-4479-8E98-4A84FD6457B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30990" yWindow="3720" windowWidth="20895" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="118">
   <si>
     <t>attributeName</t>
   </si>
@@ -75,9 +75,6 @@
     <t>niskin</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>NSF</t>
   </si>
   <si>
-    <t>OCE-1655686</t>
-  </si>
-  <si>
     <t>creator</t>
   </si>
   <si>
@@ -373,6 +367,21 @@
   </si>
   <si>
     <t>Distance to nearest station is greater than 2 km</t>
+  </si>
+  <si>
+    <t>OCE-2322676</t>
+  </si>
+  <si>
+    <t>date_time_utc</t>
+  </si>
+  <si>
+    <t>Joanne</t>
+  </si>
+  <si>
+    <t>Koch</t>
+  </si>
+  <si>
+    <t>jkoch@whoi.edu</t>
   </si>
 </sst>
 </file>
@@ -717,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,19 +765,19 @@
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -776,7 +785,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -785,7 +794,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -796,7 +805,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -805,7 +814,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -813,42 +822,42 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
@@ -856,19 +865,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -876,19 +885,19 @@
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
         <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -896,10 +905,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -908,7 +917,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
@@ -916,39 +925,39 @@
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -956,19 +965,19 @@
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -976,19 +985,19 @@
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -996,19 +1005,19 @@
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -1016,82 +1025,82 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1115,43 +1124,43 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
         <v>85</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1161,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,231 +1186,258 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>59</v>
-      </c>
-      <c r="J1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>65</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
         <v>66</v>
       </c>
-      <c r="G2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" t="s">
-        <v>67</v>
-      </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>62</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>63</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>65</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
         <v>66</v>
       </c>
-      <c r="G3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" t="s">
-        <v>67</v>
-      </c>
       <c r="J3" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" t="s">
         <v>109</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I6" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" t="s">
-        <v>74</v>
-      </c>
       <c r="H7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>93</v>
       </c>
-      <c r="D8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="G8" t="s">
         <v>94</v>
       </c>
-      <c r="F8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" t="s">
-        <v>96</v>
-      </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E8" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{3EEC4E1A-6ABB-4E77-B8C4-9878C1BE7468}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{88CCFB14-3923-4622-AF85-0EE4D575155D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1422,106 +1458,106 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new flags from API
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-nutrient-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8CF89C-18C3-4479-8E98-4A84FD6457B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBDCAF4-FE05-4F8A-A76F-9FF04F58D450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30990" yWindow="3720" windowWidth="20895" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34140" yWindow="3735" windowWidth="21600" windowHeight="12525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="129">
   <si>
     <t>attributeName</t>
   </si>
@@ -234,9 +234,6 @@
     <t>creator</t>
   </si>
   <si>
-    <t>E. Taylor</t>
-  </si>
-  <si>
     <t>Crockford</t>
   </si>
   <si>
@@ -363,9 +360,6 @@
     <t>OOI</t>
   </si>
   <si>
-    <t>Identifier for project that funded the cruise (or sample when available)</t>
-  </si>
-  <si>
     <t>Distance to nearest station is greater than 2 km</t>
   </si>
   <si>
@@ -382,13 +376,52 @@
   </si>
   <si>
     <t>jkoch@whoi.edu</t>
+  </si>
+  <si>
+    <t>flag_nitrate_nitrite</t>
+  </si>
+  <si>
+    <t>flag_ammonium</t>
+  </si>
+  <si>
+    <t>flag_phosphate</t>
+  </si>
+  <si>
+    <t>flag_silicate</t>
+  </si>
+  <si>
+    <t>Identifier for project that funded the cruise or sample</t>
+  </si>
+  <si>
+    <t>IODE Quality Flag primary level</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>quality not evaluated, not available or unknown</t>
+  </si>
+  <si>
+    <t>questionable/suspect</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>E.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Taylor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +444,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -429,11 +482,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -443,10 +499,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{A4627565-E020-486A-AC10-E5F4201BFA71}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{69DAC453-13A4-411B-9AC6-4579F8AF1CAD}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{B41CEB21-FC2C-4DEF-9A9A-C81C94085E49}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -724,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A20" sqref="A20:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,13 +831,13 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -822,25 +882,25 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -883,78 +943,78 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G9" t="s">
-        <v>8</v>
+      <c r="G9" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
         <v>30</v>
@@ -965,142 +1025,186 @@
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+      <c r="F12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D16" t="s">
         <v>31</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F16" t="s">
         <v>30</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F17" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>112</v>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1111,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,43 +1228,263 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
         <v>80</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="5">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="5">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="5">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="5">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="5">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="5">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="5">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="5">
+        <v>2</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="5">
+        <v>4</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="5">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1173,7 +1497,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1245,7 +1569,7 @@
         <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1268,7 +1592,7 @@
         <v>65</v>
       </c>
       <c r="G3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H3" t="s">
         <v>63</v>
@@ -1277,21 +1601,24 @@
         <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" t="s">
         <v>68</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
       </c>
       <c r="D4" t="s">
         <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
         <v>67</v>
@@ -1303,21 +1630,21 @@
         <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
         <v>102</v>
-      </c>
-      <c r="C5" t="s">
-        <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G5" t="s">
         <v>67</v>
@@ -1329,44 +1656,44 @@
         <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
         <v>106</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="G6" t="s">
         <v>67</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I6" t="s">
         <v>66</v>
       </c>
       <c r="J6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
         <v>63</v>
       </c>
       <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
         <v>71</v>
-      </c>
-      <c r="G7" t="s">
-        <v>72</v>
       </c>
       <c r="H7" t="s">
         <v>63</v>
@@ -1375,27 +1702,27 @@
         <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
         <v>90</v>
-      </c>
-      <c r="C8" t="s">
-        <v>91</v>
       </c>
       <c r="D8" t="s">
         <v>63</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
         <v>92</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>93</v>
-      </c>
-      <c r="G8" t="s">
-        <v>94</v>
       </c>
       <c r="H8" t="s">
         <v>63</v>
@@ -1404,24 +1731,24 @@
         <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H9" t="s">
         <v>63</v>
@@ -1430,7 +1757,7 @@
         <v>66</v>
       </c>
       <c r="J9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1466,7 +1793,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
handle duplicate sample IDs & values
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBDCAF4-FE05-4F8A-A76F-9FF04F58D450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1970E44-AB2F-4381-85A2-9053BE6AC3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34140" yWindow="3735" windowWidth="21600" windowHeight="12525" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45045" yWindow="1605" windowWidth="11985" windowHeight="13065" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="130">
   <si>
     <t>attributeName</t>
   </si>
@@ -415,6 +415,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Taylor</t>
+  </si>
+  <si>
+    <t>NSF Ocean Observatories Initiative</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1500,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1664,7 +1667,7 @@
         <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
include data table corrections, methods edits, add orcids
</commit_message>
<xml_diff>
--- a/nutrient-transect-info.xlsx
+++ b/nutrient-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmorkeski\Documents\nes-lter-nutrient-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1970E44-AB2F-4381-85A2-9053BE6AC3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C832F2C6-B702-4E46-BF15-E5A5DAE01CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45045" yWindow="1605" windowWidth="11985" windowHeight="13065" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="132">
   <si>
     <t>attributeName</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>NSF Ocean Observatories Initiative</t>
+  </si>
+  <si>
+    <t>0000-0002-2122-0462</t>
+  </si>
+  <si>
+    <t>0000-0003-0194-7282</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1506,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1508,6 +1514,7 @@
     <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.109375" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
     <col min="8" max="8" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1623,6 +1630,9 @@
       <c r="E4" t="s">
         <v>100</v>
       </c>
+      <c r="F4" t="s">
+        <v>130</v>
+      </c>
       <c r="G4" t="s">
         <v>67</v>
       </c>
@@ -1648,6 +1658,9 @@
       </c>
       <c r="E5" t="s">
         <v>99</v>
+      </c>
+      <c r="F5" t="s">
+        <v>131</v>
       </c>
       <c r="G5" t="s">
         <v>67</v>

</xml_diff>